<commit_message>
Update NB3 Body (for servo drive)
</commit_message>
<xml_diff>
--- a/boxes/electrons/NB3_body/NB3_body.xlsx
+++ b/boxes/electrons/NB3_body/NB3_body.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Unit Price</t>
   </si>
   <si>
-    <t xml:space="preserve">J10,J12,J11</t>
+    <t xml:space="preserve">J16,J15,J10,J12,J11</t>
   </si>
   <si>
     <t xml:space="preserve">Header Breakaway 6 2 Surface Mount 0.100"(2.54mm) SMD P=2.54mm Male</t>
@@ -115,6 +115,7 @@
       <sz val="10"/>
       <name val="Noto Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -206,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,6 +230,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -311,20 +316,20 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="71.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="71.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.23"/>
   </cols>
   <sheetData>
@@ -356,9 +361,9 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -473,7 +478,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Nimbus Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Nimbus Sans,Regular"Page &amp;P</oddFooter>

</xml_diff>